<commit_message>
adding Following new scripts implementation, 1.User own profile comments test 2.Others Profile comments test
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>TCID</t>
   </si>
@@ -120,14 +120,28 @@
 4.Terms of Use</t>
   </si>
   <si>
+    <t>OwnProfileCommentsLikeTest</t>
+  </si>
+  <si>
+    <t>Validate User Own Profile Comments Like Test</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>OthersProfileCommentsLikeTest</t>
+  </si>
+  <si>
+    <t>Validate Other User Profile Comments Like Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -524,18 +538,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -560,7 +574,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>26</v>
@@ -574,7 +588,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>26</v>
@@ -588,7 +602,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
@@ -602,7 +616,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>26</v>
@@ -615,8 +629,8 @@
       <c r="B6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>3</v>
+      <c r="C6" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>26</v>
@@ -630,10 +644,38 @@
         <v>30</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -651,10 +693,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -698,11 +740,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
added following new profile script 1.Profile Interest and Skills Update
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="40">
   <si>
     <t>TCID</t>
   </si>
@@ -137,11 +137,21 @@
   <si>
     <t>Validate Other User Profile Comments Like Test</t>
   </si>
+  <si>
+    <t>ProfileInterestSkillsUpdateTest</t>
+  </si>
+  <si>
+    <t>To verify User can able to update his Own Profile Interests and Skills</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -538,18 +548,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -658,10 +668,10 @@
         <v>32</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -672,9 +682,23 @@
         <v>36</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -693,10 +717,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -740,11 +764,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
Following new script automation has been done 1.follow other user's profile and validate following count got increased
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>TCID</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>To verify User can able to update his Own Profile Interests and Skills</t>
+  </si>
+  <si>
+    <t>ProfileFollowingOthersTest</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>To verity User Own Profile following other profile and following size count get increased</t>
   </si>
 </sst>
 </file>
@@ -538,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -573,7 +582,7 @@
       <c r="B2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -587,7 +596,7 @@
       <c r="B3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -601,7 +610,7 @@
       <c r="B4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -615,7 +624,7 @@
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -629,7 +638,7 @@
       <c r="B6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -643,7 +652,7 @@
       <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -657,7 +666,7 @@
       <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -671,7 +680,7 @@
       <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -685,15 +694,30 @@
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="11" spans="1:4" ht="30">
+      <c r="A11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
adding two nee testcases profilefollwertest.java profilesummarytest.java
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>TCID</t>
   </si>
@@ -147,6 +147,18 @@
     <t>To verity User Own Profile following other profile and following size count get increased</t>
   </si>
   <si>
+    <t>Add summary validation</t>
+  </si>
+  <si>
+    <t>ProfileSummaryTest</t>
+  </si>
+  <si>
+    <t>ProfileFollowerTest</t>
+  </si>
+  <si>
+    <t>To verify count of users following me</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
 </sst>
@@ -154,7 +166,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -551,18 +562,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -587,7 +598,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>26</v>
@@ -601,7 +612,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>26</v>
@@ -615,7 +626,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
@@ -629,7 +640,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>26</v>
@@ -643,7 +654,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>26</v>
@@ -657,7 +668,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>26</v>
@@ -671,7 +682,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>26</v>
@@ -685,7 +696,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
@@ -699,7 +710,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>26</v>
@@ -713,11 +724,35 @@
         <v>39</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -735,10 +770,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -782,11 +817,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
Running Whole D Suite
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>TCID</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -598,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>26</v>
@@ -612,7 +609,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>26</v>
@@ -626,7 +623,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
@@ -640,7 +637,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>26</v>
@@ -654,7 +651,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>26</v>
@@ -668,7 +665,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>26</v>
@@ -682,7 +679,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>26</v>
@@ -696,7 +693,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
@@ -710,7 +707,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>26</v>
@@ -724,7 +721,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>26</v>
@@ -738,7 +735,7 @@
         <v>39</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
running D and C suites
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>TCID</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>To verify count of users following me</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -732,7 +735,7 @@
         <v>39</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
running profile test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>TCID</t>
   </si>
@@ -155,15 +155,11 @@
   <si>
     <t>To verify count of users following me</t>
   </si>
-  <si>
-    <t>N</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -563,15 +559,15 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -736,7 +732,7 @@
         <v>39</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>26</v>
@@ -772,10 +768,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -819,11 +815,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
running all profile testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>TCID</t>
   </si>
@@ -156,9 +156,6 @@
     <t>To verify count of users following me</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
 </sst>
@@ -166,7 +163,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -566,15 +562,15 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -599,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>26</v>
@@ -613,7 +609,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>26</v>
@@ -627,7 +623,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
@@ -644,7 +640,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="90">
@@ -655,7 +651,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>26</v>
@@ -669,7 +665,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>26</v>
@@ -683,7 +679,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>26</v>
@@ -697,7 +693,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
@@ -711,7 +707,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>26</v>
@@ -725,7 +721,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>26</v>
@@ -739,7 +735,7 @@
         <v>39</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>26</v>
@@ -753,7 +749,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>26</v>
@@ -775,10 +771,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -822,11 +818,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
Added new profile search test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>TCID</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>To verity user is able to update his own profile data</t>
-  </si>
-  <si>
-    <t>SKIP</t>
   </si>
   <si>
     <t>ApplicationLinksValidationTest</t>
@@ -156,14 +153,40 @@
     <t>To verify count of users following me</t>
   </si>
   <si>
+    <t>FindProfileWithLastNameTest</t>
+  </si>
+  <si>
+    <t>Verify that user is able to find other profiles with their last name</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FindProfileWithRoleTest</t>
+  </si>
+  <si>
+    <t>Verify that user is able to find other profiles with their Title/Role</t>
+  </si>
+  <si>
+    <t>FindProfileWithPrimaryInstitutionTest</t>
+  </si>
+  <si>
+    <t>Verify that user is able to find other profiles with their Primary Institution</t>
+  </si>
+  <si>
+    <t>FindProfileWithCountryTest</t>
+  </si>
+  <si>
+    <t>Verify that user is able to find other profiles with their Country</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -560,18 +583,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -599,7 +622,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30">
@@ -613,7 +636,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -627,7 +650,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -641,119 +664,175 @@
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="90">
       <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="75">
       <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="C7" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C8" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C9" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C10" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30">
       <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="C11" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>26</v>
+      <c r="B14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -772,10 +851,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -819,11 +898,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
running all profile test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>TCID</t>
   </si>
@@ -181,9 +181,6 @@
   </si>
   <si>
     <t>Verify that user is able to find other profiles with their Country</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -589,7 +586,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -636,7 +633,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>44</v>
@@ -650,7 +647,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>44</v>
@@ -664,7 +661,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>44</v>
@@ -678,7 +675,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>44</v>
@@ -692,7 +689,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>44</v>
@@ -706,7 +703,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>44</v>
@@ -720,7 +717,7 @@
         <v>33</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>44</v>
@@ -734,7 +731,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>44</v>
@@ -748,7 +745,7 @@
         <v>37</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>44</v>
@@ -762,7 +759,7 @@
         <v>38</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>44</v>
@@ -776,7 +773,7 @@
         <v>41</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>44</v>
@@ -790,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>44</v>
@@ -804,7 +801,7 @@
         <v>47</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>44</v>
@@ -818,7 +815,7 @@
         <v>49</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>45</v>
@@ -832,7 +829,7 @@
         <v>51</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
profile scipts changes are added
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="65">
   <si>
     <t>TCID</t>
   </si>
@@ -24,9 +24,6 @@
   </si>
   <si>
     <t>Runmode</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
   <si>
     <t>Results</t>
@@ -119,9 +116,6 @@
 4.Terms of Use</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>Verify that user is able to search for profiles with interests and Skills</t>
   </si>
   <si>
@@ -133,10 +127,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">
-Verify that user is able to test for count of users following me</t>
-  </si>
-  <si>
     <t>Verify that user is able to Start/Stop following a user from profile search results page</t>
   </si>
   <si>
@@ -151,15 +141,90 @@
     <t>Verify that user is able to edit  info like Interests and Skills from his own profile</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that user is able to edit Summary field from his own profile and validate max length condition
-</t>
-  </si>
-  <si>
     <t>Verify that user is able to Start/Stop following a user from profile page 
 Verify that user should not able to  Edit others profile</t>
   </si>
   <si>
     <t>Verify that user is able to edit  info like title/role,Primary Institution and country from his own profile</t>
+  </si>
+  <si>
+    <t>OPQA-444</t>
+  </si>
+  <si>
+    <t>OPQA-445|OPQA-711</t>
+  </si>
+  <si>
+    <t>OPQA-494|OPQA-501</t>
+  </si>
+  <si>
+    <t>OPQA-495</t>
+  </si>
+  <si>
+    <t>OPQA-498</t>
+  </si>
+  <si>
+    <t>OPQA-499</t>
+  </si>
+  <si>
+    <t>OPQA-496</t>
+  </si>
+  <si>
+    <t>OPQA-447</t>
+  </si>
+  <si>
+    <t>Verify that user is able to edit Summary field from his own profile and validate max length condition</t>
+  </si>
+  <si>
+    <t>OPQA-497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Verify that user is able to test for count of users I am following</t>
+  </si>
+  <si>
+    <t>OPQA-446</t>
+  </si>
+  <si>
+    <t>OPQA-437</t>
+  </si>
+  <si>
+    <t>OPQA-439</t>
+  </si>
+  <si>
+    <t>OPQA-441</t>
+  </si>
+  <si>
+    <t>OPQA-440</t>
+  </si>
+  <si>
+    <t>OPQA-438</t>
+  </si>
+  <si>
+    <t>OPQA-742</t>
+  </si>
+  <si>
+    <t>OPQA-743</t>
+  </si>
+  <si>
+    <t>JIRA ID</t>
+  </si>
+  <si>
+    <t>OPQA-444|OPQA-434</t>
+  </si>
+  <si>
+    <t>OPQA-445|OPQA-711|OPQA-435|OPQA-436</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -237,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -260,6 +325,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,270 +626,377 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="36.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30">
       <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30">
+      <c r="A5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="90">
+      <c r="A6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="90">
+      <c r="A7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30">
+      <c r="A8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30">
+      <c r="A10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="D10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45">
+      <c r="A11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30">
+      <c r="A12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30">
+      <c r="A13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="30">
-      <c r="A3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30">
-      <c r="A4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30">
-      <c r="A5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="90">
-      <c r="A6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="90">
-      <c r="A7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="B15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75">
+      <c r="A18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30">
-      <c r="A8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30">
-      <c r="A9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30">
-      <c r="A10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45">
-      <c r="A11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="60">
-      <c r="A12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30">
-      <c r="A13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75">
-      <c r="A18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>21</v>
+      <c r="D18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -852,10 +1026,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="48" customHeight="1">

</xml_diff>

<commit_message>
code changes done profile scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -127,9 +127,6 @@
 </t>
   </si>
   <si>
-    <t>Verify that user is able to Start/Stop following a user from profile search results page</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that user is able to Like his own comments from his profile page 
 </t>
   </si>
@@ -216,6 +213,10 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>Verify that user is able to Start/Stop following a user from profile search results page
+Verify that user is able to search for profiles</t>
   </si>
 </sst>
 </file>
@@ -618,7 +619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -637,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -649,15 +650,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30">
+    <row r="2" spans="1:6" ht="45">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>59</v>
@@ -672,13 +673,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>20</v>
@@ -690,13 +691,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>20</v>
@@ -708,13 +709,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>20</v>
@@ -726,7 +727,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>28</v>
@@ -735,7 +736,7 @@
         <v>59</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="F6" s="10"/>
     </row>
@@ -744,13 +745,13 @@
         <v>11</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>20</v>
@@ -762,13 +763,13 @@
         <v>12</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>20</v>
@@ -780,13 +781,13 @@
         <v>13</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>20</v>
@@ -798,13 +799,13 @@
         <v>14</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>20</v>
@@ -816,13 +817,13 @@
         <v>15</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>20</v>
@@ -834,13 +835,13 @@
         <v>16</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>20</v>
@@ -852,10 +853,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>59</v>
@@ -870,16 +871,16 @@
         <v>18</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="F14" s="10"/>
     </row>
@@ -888,16 +889,16 @@
         <v>21</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="F15" s="10"/>
     </row>
@@ -906,13 +907,13 @@
         <v>23</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>20</v>
@@ -924,13 +925,13 @@
         <v>25</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>20</v>
@@ -942,13 +943,13 @@
         <v>27</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>30</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
running D suite testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
adding new profile test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -232,7 +232,7 @@
     <t>OtherProfilePageFollowTest</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -780,7 +780,7 @@
         <v>55</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="F7" s="11"/>
     </row>
@@ -870,7 +870,7 @@
         <v>55</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="F12" s="11"/>
     </row>

</xml_diff>

<commit_message>
running specific profile testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
   <si>
     <t>TCID</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -645,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -687,7 +690,7 @@
         <v>56</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>20</v>
@@ -705,7 +708,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>20</v>
@@ -723,7 +726,7 @@
         <v>59</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>20</v>
@@ -741,7 +744,7 @@
         <v>62</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>20</v>
@@ -759,7 +762,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>20</v>
@@ -777,7 +780,7 @@
         <v>35</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>20</v>
@@ -795,7 +798,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>20</v>
@@ -813,7 +816,7 @@
         <v>57</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>20</v>
@@ -831,7 +834,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>20</v>
@@ -849,7 +852,7 @@
         <v>33</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>20</v>
@@ -885,7 +888,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>20</v>
@@ -903,7 +906,7 @@
         <v>42</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>20</v>
@@ -939,7 +942,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>20</v>
@@ -957,7 +960,7 @@
         <v>22</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>20</v>
@@ -975,7 +978,7 @@
         <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>20</v>
@@ -993,7 +996,7 @@
         <v>26</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>20</v>
@@ -1011,7 +1014,7 @@
         <v>29</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
added jira id for D suite
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -146,9 +146,6 @@
     <t>OPQA-499</t>
   </si>
   <si>
-    <t>OPQA-496</t>
-  </si>
-  <si>
     <t>OPQA-447</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>OPQA-496|OPQA-511</t>
   </si>
 </sst>
 </file>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -664,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -681,13 +681,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>20</v>
@@ -699,13 +699,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>20</v>
@@ -714,16 +714,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>20</v>
@@ -732,16 +732,16 @@
     </row>
     <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>20</v>
@@ -759,7 +759,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>20</v>
@@ -777,7 +777,7 @@
         <v>35</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>20</v>
@@ -789,13 +789,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>20</v>
@@ -807,13 +807,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>20</v>
@@ -831,7 +831,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>20</v>
@@ -849,7 +849,7 @@
         <v>33</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>20</v>
@@ -861,16 +861,16 @@
         <v>14</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12" s="11"/>
     </row>
@@ -879,13 +879,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>20</v>
@@ -897,13 +897,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>20</v>
@@ -915,13 +915,13 @@
         <v>17</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>20</v>
@@ -933,13 +933,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>20</v>
@@ -951,13 +951,13 @@
         <v>21</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>20</v>
@@ -969,13 +969,13 @@
         <v>23</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>20</v>
@@ -987,13 +987,13 @@
         <v>25</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>20</v>
@@ -1005,13 +1005,13 @@
         <v>27</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
taking the latest update
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
   <si>
     <t>TCID</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Verify that user is able to find other profiles with their last name</t>
-  </si>
-  <si>
-    <t>SKIP</t>
   </si>
   <si>
     <t>FindProfileWithRoleTest</t>
@@ -189,9 +186,6 @@
     <t>OPQA-444|OPQA-434</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Verify that user is able to Start/Stop following a user from profile search results page
 Verify that user is able to search for profiles</t>
   </si>
@@ -229,9 +223,6 @@
     <t>OtherProfilePageFollowTest</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>OPQA-496|OPQA-511</t>
   </si>
   <si>
@@ -260,6 +251,33 @@
   </si>
   <si>
     <t>OPQA-508</t>
+  </si>
+  <si>
+    <t>ProfilePostsValidationTest</t>
+  </si>
+  <si>
+    <t>OPQA-514</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user is able to see all his POST's from his profile page. </t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>AddPostToWatchlistTest</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add his Post to 'watchlist'  from his profile.</t>
+  </si>
+  <si>
+    <t>OPQA-515</t>
   </si>
 </sst>
 </file>
@@ -691,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D23"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,7 +730,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -729,16 +747,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F2" s="10"/>
     </row>
@@ -747,52 +765,52 @@
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F5" s="10"/>
     </row>
@@ -801,16 +819,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F6" s="10"/>
     </row>
@@ -819,16 +837,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F7" s="11"/>
     </row>
@@ -837,16 +855,16 @@
         <v>10</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -855,16 +873,16 @@
         <v>11</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F9" s="10"/>
     </row>
@@ -873,16 +891,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F10" s="10"/>
     </row>
@@ -891,16 +909,16 @@
         <v>13</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F11" s="10"/>
     </row>
@@ -909,16 +927,16 @@
         <v>14</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F12" s="11"/>
     </row>
@@ -927,16 +945,16 @@
         <v>15</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F13" s="10"/>
     </row>
@@ -945,16 +963,16 @@
         <v>16</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F14" s="10"/>
     </row>
@@ -963,16 +981,16 @@
         <v>17</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F15" s="10"/>
     </row>
@@ -981,140 +999,174 @@
         <v>18</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="15.75">
       <c r="A20" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="31.5">
       <c r="A22" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75">
       <c r="A23" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75">
+      <c r="A24" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B24" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>65</v>
+      <c r="D24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes done in D suite.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="92">
   <si>
     <t>TCID</t>
   </si>
@@ -275,9 +275,6 @@
   </si>
   <si>
     <t>ProfilePrimaryInstitutionTypeAheadTest</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>Verify that user is able to add 'primary institution' using type ahead</t>
@@ -368,6 +365,18 @@
       </rPr>
       <t xml:space="preserve"> using type ahead options should display while enter min 2 characters</t>
     </r>
+  </si>
+  <si>
+    <t>OPQA-512</t>
+  </si>
+  <si>
+    <t>OPQA-516</t>
+  </si>
+  <si>
+    <t>OPQA-517</t>
+  </si>
+  <si>
+    <t>OPQA-518</t>
   </si>
 </sst>
 </file>
@@ -793,7 +802,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1255,10 +1264,10 @@
         <v>80</v>
       </c>
       <c r="B26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>82</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>75</v>
@@ -1269,13 +1278,13 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>75</v>
@@ -1286,13 +1295,13 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>75</v>
@@ -1303,13 +1312,13 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>88</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
Commit for D suite Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="92">
   <si>
     <t>TCID</t>
   </si>
@@ -275,9 +275,6 @@
   </si>
   <si>
     <t>ProfilePrimaryInstitutionTypeAheadTest</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>Verify that user is able to add 'primary institution' using type ahead</t>
@@ -368,6 +365,18 @@
       </rPr>
       <t xml:space="preserve"> using type ahead options should display while enter min 2 characters</t>
     </r>
+  </si>
+  <si>
+    <t>OPQA-512</t>
+  </si>
+  <si>
+    <t>OPQA-516</t>
+  </si>
+  <si>
+    <t>OPQA-517</t>
+  </si>
+  <si>
+    <t>OPQA-518</t>
   </si>
 </sst>
 </file>
@@ -793,7 +802,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1255,10 +1264,10 @@
         <v>80</v>
       </c>
       <c r="B26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>82</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>75</v>
@@ -1269,13 +1278,13 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>75</v>
@@ -1286,13 +1295,13 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>75</v>
@@ -1303,13 +1312,13 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>88</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
code changes are done in Xls_Reader.java
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/D suite.xlsx
+++ b/src/test/resources/xls/D suite.xlsx
@@ -581,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -595,8 +595,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -907,11 +905,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" activeCellId="4" sqref="C34 C34 C34 C34 C34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -920,10 +916,9 @@
     <col min="3" max="3" width="87.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="36.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -940,7 +935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30">
+    <row r="2" spans="1:5" ht="30">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -956,9 +951,8 @@
       <c r="E2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" ht="30">
+    </row>
+    <row r="3" spans="1:5" ht="30">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -974,9 +968,8 @@
       <c r="E3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>53</v>
       </c>
@@ -992,16 +985,15 @@
       <c r="E4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75">
+    </row>
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1010,9 +1002,8 @@
       <c r="E5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" ht="30">
+    </row>
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1028,9 +1019,8 @@
       <c r="E6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" ht="30">
+    </row>
+    <row r="7" spans="1:5" ht="30">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1046,9 +1036,8 @@
       <c r="E7" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" ht="90">
+    </row>
+    <row r="8" spans="1:5" ht="90">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1064,9 +1053,8 @@
       <c r="E8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="90">
+    </row>
+    <row r="9" spans="1:5" ht="90">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1082,9 +1070,8 @@
       <c r="E9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="30">
+    </row>
+    <row r="10" spans="1:5" ht="30">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1100,9 +1087,8 @@
       <c r="E10" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" ht="30">
+    </row>
+    <row r="11" spans="1:5" ht="30">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -1118,9 +1104,8 @@
       <c r="E11" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -1136,9 +1121,8 @@
       <c r="E12" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" ht="30">
+    </row>
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1154,9 +1138,8 @@
       <c r="E13" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" ht="30">
+    </row>
+    <row r="14" spans="1:5" ht="30">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
@@ -1172,9 +1155,8 @@
       <c r="E14" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" ht="30">
+    </row>
+    <row r="15" spans="1:5" ht="30">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -1190,9 +1172,8 @@
       <c r="E15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6">
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1208,9 +1189,8 @@
       <c r="E16" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -1226,9 +1206,8 @@
       <c r="E17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6">
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
@@ -1244,9 +1223,8 @@
       <c r="E18" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
@@ -1262,9 +1240,8 @@
       <c r="E19" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75">
+    </row>
+    <row r="20" spans="1:5" ht="15.75">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1280,362 +1257,361 @@
       <c r="E20" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="10" t="s">
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>63</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75">
-      <c r="A22" s="10" t="s">
+      <c r="E21" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75">
+      <c r="A22" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75">
-      <c r="A23" s="10" t="s">
+      <c r="E22" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75">
+      <c r="A23" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="11" t="s">
         <v>69</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75">
-      <c r="A24" s="10" t="s">
+      <c r="E23" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75">
+      <c r="A24" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="10" t="s">
+      <c r="E24" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="8" t="s">
         <v>77</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="10" t="s">
+      <c r="E25" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="10" t="s">
+      <c r="E26" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="10" t="s">
+      <c r="E27" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E28" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="10" t="s">
+      <c r="E28" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="8" t="s">
         <v>87</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="10" t="s">
+      <c r="E29" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="8" t="s">
         <v>93</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="10" t="s">
+      <c r="E30" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="8" t="s">
         <v>95</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E31" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="10" t="s">
+      <c r="E31" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="8" t="s">
         <v>97</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="8" t="s">
         <v>99</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="8" t="s">
         <v>101</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="8" t="s">
         <v>103</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="8" t="s">
         <v>104</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="8" t="s">
         <v>107</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="8" t="s">
         <v>109</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="8" t="s">
         <v>111</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="8" t="s">
         <v>115</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="8" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>